<commit_message>
adding import Excel ListeAdmis
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9876"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9876" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="gege" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -50,7 +51,10 @@
     <t>insert</t>
   </si>
   <si>
-    <t>Autre</t>
+    <t>DJ</t>
+  </si>
+  <si>
+    <t>VAOVAO</t>
   </si>
 </sst>
 </file>
@@ -370,8 +374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,6 +420,63 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>

</xml_diff>